<commit_message>
Dopisałem się do sprinta. K Ziel
</commit_message>
<xml_diff>
--- a/Sprint_1.xlsx
+++ b/Sprint_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BiomedEKG\BiomedEKG\ecg_holter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dadm\ecg_holter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
   <si>
     <t>Software architect</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>Ile czasu poświęcono</t>
+  </si>
+  <si>
+    <t>Diagramy klas, ogarnięcie pojawiajacych się problemów z postawieniem projektu, opieprzanie Pauliny za inicjatywę godną rzodkiewki.</t>
+  </si>
+  <si>
+    <t>postawiłem projekt!</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>3/4dni</t>
   </si>
 </sst>
 </file>
@@ -843,7 +855,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,8 +863,8 @@
     <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="71" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
@@ -912,10 +924,18 @@
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
+      <c r="D4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">

</xml_diff>